<commit_message>
Updated all marksheets and merged with documents
</commit_message>
<xml_diff>
--- a/Marksheets/Abhisekh Lamichhane.xlsx
+++ b/Marksheets/Abhisekh Lamichhane.xlsx
@@ -286,10 +286,6 @@
     <t>very poorly written code and no comments at all</t>
   </si>
   <si>
-    <t xml:space="preserve">In overall the code is working and all the functionality seems working and system can be used 
-</t>
-  </si>
-  <si>
     <t>Very poor code</t>
   </si>
   <si>
@@ -313,11 +309,21 @@
   <si>
     <t>Total Marks</t>
   </si>
+  <si>
+    <t xml:space="preserve">In overall the code is working and all the functionality seems working and system can be used. All feature implemented with few minor bugs
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="27">
     <font>
       <sz val="11"/>
@@ -1134,9 +1140,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1204,6 +1207,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1620,7 +1626,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
-      <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="E18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
       <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
@@ -2137,11 +2143,11 @@
       </c>
       <c r="E13" s="31" t="str">
         <f>G13</f>
-        <v>Excellent report presentation in tabular format with proper chart for enrollment and weekly report for selected week </v>
+        <v>Excellent report presentation in tabular format with proper chart for enrollment and weekly report for selected week</v>
       </c>
       <c r="F13" s="31" t="str">
         <f>G13</f>
-        <v>Excellent report presentation in tabular format with proper chart for enrollment and weekly report for selected week </v>
+        <v>Excellent report presentation in tabular format with proper chart for enrollment and weekly report for selected week</v>
       </c>
       <c r="G13" s="31" t="s">
         <v>42</v>
@@ -2364,7 +2370,7 @@
       </c>
       <c r="H18" s="44" t="str">
         <f>I18</f>
-        <v>User Manual is good. Contains all varieties of forms. </v>
+        <v>User Manual is good. Contains all varieties of forms.</v>
       </c>
       <c r="I18" s="44" t="s">
         <v>61</v>
@@ -2378,14 +2384,14 @@
       </c>
       <c r="L18" s="44" t="str">
         <f>M18</f>
-        <v>User Manual is below average. Is textual only. </v>
+        <v>User Manual is below average. Is textual only.</v>
       </c>
       <c r="M18" s="44" t="s">
         <v>63</v>
       </c>
       <c r="N18" s="44" t="str">
         <f>M18</f>
-        <v>User Manual is below average. Is textual only. </v>
+        <v>User Manual is below average. Is textual only.</v>
       </c>
       <c r="O18" s="45" t="s">
         <v>29</v>
@@ -2604,7 +2610,7 @@
       </c>
       <c r="N23" s="62"/>
       <c r="O23" s="64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P23" s="65"/>
       <c r="Q23" s="65"/>
@@ -2623,7 +2629,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="68">
         <v>5</v>
@@ -2634,23 +2640,23 @@
       <c r="E24" s="70"/>
       <c r="F24" s="70"/>
       <c r="G24" s="71" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H24" s="70"/>
       <c r="I24" s="71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J24" s="70"/>
       <c r="K24" s="71" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L24" s="70"/>
       <c r="M24" s="71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N24" s="70"/>
       <c r="O24" s="72" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P24" s="65"/>
       <c r="Q24" s="65"/>
@@ -2667,7 +2673,7 @@
     <row r="25" spans="1:26" ht="14.25" customHeight="1">
       <c r="A25" s="73"/>
       <c r="B25" s="74" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" s="74">
         <f t="shared" si="6" ref="C25:D25">SUM(C10:C24)</f>
@@ -30014,22 +30020,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A55">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="24.25390625" customWidth="1"/>
     <col min="2" max="2" width="19.125" customWidth="1"/>
-    <col min="3" max="3" width="2.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.75390625" customWidth="1"/>
     <col min="4" max="4" width="26.625" customWidth="1"/>
     <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
     <col min="6" max="26" width="7.75390625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="33" customHeight="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="100" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="79"/>
@@ -30059,7 +30065,7 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="102"/>
+      <c r="A2" s="101"/>
       <c r="B2" s="79"/>
       <c r="C2" s="79"/>
       <c r="D2" s="79"/>
@@ -30115,7 +30121,7 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="18">
-      <c r="A4" s="103" t="str">
+      <c r="A4" s="102" t="str">
         <f>'Grading Sheet'!B4</f>
         <v>Application Development</v>
       </c>
@@ -30146,7 +30152,7 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A5" s="103" t="str">
+      <c r="A5" s="102" t="str">
         <f>'Grading Sheet'!B3</f>
         <v>CS6004NI</v>
       </c>
@@ -30177,7 +30183,7 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="27" customHeight="1">
-      <c r="A6" s="98" t="s">
+      <c r="A6" s="97" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="79"/>
@@ -30638,7 +30644,7 @@
     <row r="22" spans="1:26" ht="14.25" customHeight="1">
       <c r="A22" s="76" t="str">
         <f>"London Met ID: "</f>
-        <v>London Met ID: </v>
+        <v>London Met ID:</v>
       </c>
       <c r="B22" s="25">
         <f>'Grading Sheet'!C7</f>
@@ -31044,13 +31050,13 @@
       <c r="Z36" s="3"/>
     </row>
     <row r="37" spans="1:26" ht="53.25" customHeight="1">
-      <c r="A37" s="104" t="s">
+      <c r="A37" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="105"/>
-      <c r="C37" s="105"/>
-      <c r="D37" s="105"/>
-      <c r="E37" s="106"/>
+      <c r="B37" s="104"/>
+      <c r="C37" s="104"/>
+      <c r="D37" s="104"/>
+      <c r="E37" s="105"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -31074,14 +31080,14 @@
       <c r="Z37" s="3"/>
     </row>
     <row r="38" spans="1:26" ht="30.75" customHeight="1">
-      <c r="A38" s="88" t="str">
+      <c r="A38" s="87" t="str">
         <f>CONCATENATE('Grading Sheet'!A9,". ",'Grading Sheet'!B9)</f>
         <v>A. Implementation of Application</v>
       </c>
-      <c r="B38" s="94"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="95"/>
+      <c r="B38" s="93"/>
+      <c r="C38" s="93"/>
+      <c r="D38" s="93"/>
+      <c r="E38" s="94"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -31105,17 +31111,17 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" spans="1:26" ht="90" customHeight="1">
-      <c r="A39" s="83" t="str">
+      <c r="A39" s="82" t="str">
         <f>'Grading Sheet'!B10</f>
         <v>User Interface and proper controls used for designing</v>
       </c>
-      <c r="B39" s="99"/>
-      <c r="C39" s="100"/>
-      <c r="D39" s="96" t="str">
+      <c r="B39" s="98"/>
+      <c r="C39" s="99"/>
+      <c r="D39" s="95" t="str">
         <f>IF('Grading Sheet'!D10&gt;'Grading Sheet'!C10*'Grading Sheet'!$G$8,'Grading Sheet'!G10,IF('Grading Sheet'!D10&gt;'Grading Sheet'!C10*'Grading Sheet'!$I$8,'Grading Sheet'!I10,IF('Grading Sheet'!D10&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C10,'Grading Sheet'!K10,IF('Grading Sheet'!D10&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C10,'Grading Sheet'!M10,'Grading Sheet'!O10))))</f>
         <v>User Interface is complete but not separated and have proper use of controls</v>
       </c>
-      <c r="E39" s="97"/>
+      <c r="E39" s="96"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -31139,17 +31145,17 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" spans="1:26" ht="90" customHeight="1">
-      <c r="A40" s="83" t="str">
+      <c r="A40" s="82" t="str">
         <f>'Grading Sheet'!B11</f>
         <v>Manual data entry or import from csv</v>
       </c>
-      <c r="B40" s="81"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="93" t="str">
+      <c r="B40" s="80"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="92" t="str">
         <f>IF('Grading Sheet'!D11&gt;'Grading Sheet'!C11*'Grading Sheet'!$G$8,'Grading Sheet'!G11,IF('Grading Sheet'!D11&gt;'Grading Sheet'!C11*'Grading Sheet'!$I$8,'Grading Sheet'!I11,IF('Grading Sheet'!D11&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C11,'Grading Sheet'!K11,IF('Grading Sheet'!D11&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C11,'Grading Sheet'!M11,'Grading Sheet'!O11))))</f>
         <v>appropriate use of data types but missing some properties required or missing CRUD operation</v>
       </c>
-      <c r="E40" s="85"/>
+      <c r="E40" s="84"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -31173,17 +31179,17 @@
       <c r="Z40" s="3"/>
     </row>
     <row r="41" spans="1:26" ht="90" customHeight="1">
-      <c r="A41" s="83" t="str">
+      <c r="A41" s="82" t="str">
         <f>'Grading Sheet'!B12</f>
         <v>Data Validation</v>
       </c>
-      <c r="B41" s="81"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="93" t="str">
+      <c r="B41" s="80"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="92" t="str">
         <f>IF('Grading Sheet'!D12&gt;'Grading Sheet'!C12*'Grading Sheet'!$G$8,'Grading Sheet'!G12,IF('Grading Sheet'!D12&gt;'Grading Sheet'!C12*'Grading Sheet'!$I$8,'Grading Sheet'!I12,IF('Grading Sheet'!D12&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C12,'Grading Sheet'!K12,IF('Grading Sheet'!D12&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C12,'Grading Sheet'!M12,'Grading Sheet'!O12))))</f>
         <v>No validation at all</v>
       </c>
-      <c r="E41" s="85"/>
+      <c r="E41" s="84"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -31207,17 +31213,17 @@
       <c r="Z41" s="3"/>
     </row>
     <row r="42" spans="1:26" ht="33" customHeight="1">
-      <c r="A42" s="83" t="str">
+      <c r="A42" s="82" t="str">
         <f>'Grading Sheet'!B13</f>
         <v>Enrollment Report &amp; weekly report in tabular format</v>
       </c>
-      <c r="B42" s="81"/>
-      <c r="C42" s="82"/>
-      <c r="D42" s="93" t="str">
+      <c r="B42" s="80"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="92" t="str">
         <f>IF('Grading Sheet'!D13&gt;'Grading Sheet'!C13*'Grading Sheet'!$G$8,'Grading Sheet'!G13,IF('Grading Sheet'!D13&gt;'Grading Sheet'!C13*'Grading Sheet'!$I$8,'Grading Sheet'!I13,IF('Grading Sheet'!D13&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C13,'Grading Sheet'!K13,IF('Grading Sheet'!D13&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C13,'Grading Sheet'!M13,'Grading Sheet'!O13))))</f>
         <v>very poorly executed reports and data not shown accurately</v>
       </c>
-      <c r="E42" s="85"/>
+      <c r="E42" s="84"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -31241,17 +31247,17 @@
       <c r="Z42" s="3"/>
     </row>
     <row r="43" spans="1:26" ht="90" customHeight="1">
-      <c r="A43" s="83" t="str">
+      <c r="A43" s="82" t="str">
         <f>'Grading Sheet'!B14</f>
         <v>Course wise enrollment report &amp; Chart display</v>
       </c>
-      <c r="B43" s="81"/>
-      <c r="C43" s="82"/>
-      <c r="D43" s="93" t="str">
+      <c r="B43" s="80"/>
+      <c r="C43" s="81"/>
+      <c r="D43" s="92" t="str">
         <f>IF('Grading Sheet'!D14&gt;'Grading Sheet'!C14*'Grading Sheet'!$G$8,'Grading Sheet'!G14,IF('Grading Sheet'!D14&gt;'Grading Sheet'!C14*'Grading Sheet'!$I$8,'Grading Sheet'!I14,IF('Grading Sheet'!D14&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C14,'Grading Sheet'!K14,IF('Grading Sheet'!D14&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C14,'Grading Sheet'!M14,'Grading Sheet'!O14))))</f>
         <v>Very poorly designed and only contains one report format with in appropriate data</v>
       </c>
-      <c r="E43" s="85"/>
+      <c r="E43" s="84"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -31275,17 +31281,17 @@
       <c r="Z43" s="3"/>
     </row>
     <row r="44" spans="1:26" ht="90" customHeight="1">
-      <c r="A44" s="83" t="str">
+      <c r="A44" s="82" t="str">
         <f>'Grading Sheet'!B15</f>
         <v>Algorithm used for sorting &amp; proper sorting of data</v>
       </c>
-      <c r="B44" s="81"/>
-      <c r="C44" s="82"/>
-      <c r="D44" s="93" t="str">
+      <c r="B44" s="80"/>
+      <c r="C44" s="81"/>
+      <c r="D44" s="92" t="str">
         <f>IF('Grading Sheet'!D15&gt;'Grading Sheet'!C15*'Grading Sheet'!$G$8,'Grading Sheet'!G15,IF('Grading Sheet'!D15&gt;'Grading Sheet'!C15*'Grading Sheet'!$I$8,'Grading Sheet'!I15,IF('Grading Sheet'!D15&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C15,'Grading Sheet'!K15,IF('Grading Sheet'!D15&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C15,'Grading Sheet'!M15,'Grading Sheet'!O15))))</f>
         <v>Sorting is implemented for not function properly</v>
       </c>
-      <c r="E44" s="85"/>
+      <c r="E44" s="84"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -31309,14 +31315,14 @@
       <c r="Z44" s="3"/>
     </row>
     <row r="45" spans="1:26" ht="33" customHeight="1">
-      <c r="A45" s="88" t="str">
+      <c r="A45" s="87" t="str">
         <f>CONCATENATE('Grading Sheet'!A17,". ",'Grading Sheet'!B17)</f>
         <v>B. Documentation</v>
       </c>
-      <c r="B45" s="81"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
+      <c r="B45" s="80"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="80"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -31340,17 +31346,17 @@
       <c r="Z45" s="3"/>
     </row>
     <row r="46" spans="1:26" ht="90" customHeight="1">
-      <c r="A46" s="83" t="str">
+      <c r="A46" s="82" t="str">
         <f>'Grading Sheet'!B18</f>
         <v>User Manual for running the application</v>
       </c>
-      <c r="B46" s="81"/>
-      <c r="C46" s="82"/>
-      <c r="D46" s="93" t="str">
+      <c r="B46" s="80"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="92" t="str">
         <f>IF('Grading Sheet'!D18&gt;'Grading Sheet'!C18*'Grading Sheet'!$G$8,'Grading Sheet'!G18,IF('Grading Sheet'!D18&gt;'Grading Sheet'!C18*'Grading Sheet'!$I$8,'Grading Sheet'!I18,IF('Grading Sheet'!D18&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C18,'Grading Sheet'!K18,IF('Grading Sheet'!D18&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C18,'Grading Sheet'!M18,'Grading Sheet'!O18))))</f>
-        <v>User Manual is good. Contains all varieties of forms. </v>
+        <v>User Manual is good. Contains all varieties of forms.</v>
       </c>
-      <c r="E46" s="85"/>
+      <c r="E46" s="84"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -31374,17 +31380,17 @@
       <c r="Z46" s="3"/>
     </row>
     <row r="47" spans="1:26" ht="90" customHeight="1">
-      <c r="A47" s="83" t="str">
+      <c r="A47" s="82" t="str">
         <f>'Grading Sheet'!B19</f>
         <v>Application architecture &amp; description of the classes ad methods sued</v>
       </c>
-      <c r="B47" s="81"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="93" t="str">
+      <c r="B47" s="80"/>
+      <c r="C47" s="81"/>
+      <c r="D47" s="92" t="str">
         <f>IF('Grading Sheet'!D19&gt;'Grading Sheet'!C19*'Grading Sheet'!$G$8,'Grading Sheet'!G19,IF('Grading Sheet'!D19&gt;'Grading Sheet'!C19*'Grading Sheet'!$I$8,'Grading Sheet'!I19,IF('Grading Sheet'!D19&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C19,'Grading Sheet'!K19,IF('Grading Sheet'!D19&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C19,'Grading Sheet'!M19,'Grading Sheet'!O19))))</f>
         <v>architecture is included and satisactory descriptoin of class and methods used.</v>
       </c>
-      <c r="E47" s="85"/>
+      <c r="E47" s="84"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -31408,17 +31414,17 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" ht="90" customHeight="1">
-      <c r="A48" s="83" t="str">
+      <c r="A48" s="82" t="str">
         <f>'Grading Sheet'!B20</f>
         <v>Flow chart, algoriathms and data sctructures used</v>
       </c>
-      <c r="B48" s="81"/>
-      <c r="C48" s="82"/>
-      <c r="D48" s="93" t="str">
+      <c r="B48" s="80"/>
+      <c r="C48" s="81"/>
+      <c r="D48" s="92" t="str">
         <f>IF('Grading Sheet'!D20&gt;'Grading Sheet'!C20*'Grading Sheet'!$G$8,'Grading Sheet'!G20,IF('Grading Sheet'!D20&gt;'Grading Sheet'!C20*'Grading Sheet'!$I$8,'Grading Sheet'!I20,IF('Grading Sheet'!D20&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C20,'Grading Sheet'!K20,IF('Grading Sheet'!D20&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C20,'Grading Sheet'!M20,'Grading Sheet'!O20))))</f>
         <v>average work with very limited explanation and missing diagramatic representation.</v>
       </c>
-      <c r="E48" s="85"/>
+      <c r="E48" s="84"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -31442,17 +31448,17 @@
       <c r="Z48" s="3"/>
     </row>
     <row r="49" spans="1:26" ht="90" customHeight="1">
-      <c r="A49" s="83" t="str">
+      <c r="A49" s="82" t="str">
         <f>'Grading Sheet'!B21</f>
         <v>Reflective essay</v>
       </c>
-      <c r="B49" s="81"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="93" t="str">
+      <c r="B49" s="80"/>
+      <c r="C49" s="81"/>
+      <c r="D49" s="92" t="str">
         <f>IF('Grading Sheet'!D21&gt;'Grading Sheet'!C21*'Grading Sheet'!$G$8,'Grading Sheet'!G21,IF('Grading Sheet'!D21&gt;'Grading Sheet'!C21*'Grading Sheet'!$I$8,'Grading Sheet'!I21,IF('Grading Sheet'!D21&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C21,'Grading Sheet'!K21,IF('Grading Sheet'!D21&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C21,'Grading Sheet'!M21,'Grading Sheet'!O21))))</f>
-        <v>satisfactorily written about experience and learnings </v>
+        <v>satisfactorily written about experience and learnings</v>
       </c>
-      <c r="E49" s="85"/>
+      <c r="E49" s="84"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -31476,14 +31482,14 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" ht="15" customHeight="1">
-      <c r="A50" s="88" t="str">
+      <c r="A50" s="87" t="str">
         <f>CONCATENATE('Grading Sheet'!A22,". ",'Grading Sheet'!B22)</f>
         <v>C. Programming Style</v>
       </c>
-      <c r="B50" s="81"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="81"/>
-      <c r="E50" s="81"/>
+      <c r="B50" s="80"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="80"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -31507,17 +31513,17 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" ht="69.75" customHeight="1">
-      <c r="A51" s="83" t="str">
+      <c r="A51" s="82" t="str">
         <f>'Grading Sheet'!B23</f>
         <v>Clarity of code,Popper Naming convention &amp; comments</v>
       </c>
-      <c r="B51" s="81"/>
-      <c r="C51" s="82"/>
-      <c r="D51" s="84" t="str">
+      <c r="B51" s="80"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="83" t="str">
         <f>IF('Grading Sheet'!D23&gt;'Grading Sheet'!C23*'Grading Sheet'!$G$8,'Grading Sheet'!G23,IF('Grading Sheet'!D23&gt;'Grading Sheet'!C23*'Grading Sheet'!$I$8,'Grading Sheet'!I23,IF('Grading Sheet'!D23&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C23,'Grading Sheet'!K23,IF('Grading Sheet'!D23&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C23,'Grading Sheet'!M23,'Grading Sheet'!O23))))</f>
-        <v>Code is poorly written and lacks comments </v>
+        <v>Code is poorly written and lacks comments</v>
       </c>
-      <c r="E51" s="85"/>
+      <c r="E51" s="84"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -31541,17 +31547,17 @@
       <c r="Z51" s="3"/>
     </row>
     <row r="52" spans="1:26" ht="81.75" customHeight="1">
-      <c r="A52" s="83" t="str">
+      <c r="A52" s="82" t="str">
         <f>'Grading Sheet'!B24</f>
         <v>System Usability</v>
       </c>
-      <c r="B52" s="81"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="84" t="str">
+      <c r="B52" s="80"/>
+      <c r="C52" s="81"/>
+      <c r="D52" s="83" t="str">
         <f>IF('Grading Sheet'!D24&gt;'Grading Sheet'!C24*'Grading Sheet'!$G$8,'Grading Sheet'!G24,IF('Grading Sheet'!D24&gt;'Grading Sheet'!C24*'Grading Sheet'!$I$8,'Grading Sheet'!I24,IF('Grading Sheet'!D24&gt;'Grading Sheet'!$K$8*'Grading Sheet'!C24,'Grading Sheet'!K24,IF('Grading Sheet'!D24&gt;'Grading Sheet'!$M$8*'Grading Sheet'!C24,'Grading Sheet'!M24,'Grading Sheet'!O24))))</f>
         <v>System can be used but is in efficient and in attracative</v>
       </c>
-      <c r="E52" s="85"/>
+      <c r="E52" s="84"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -31575,10 +31581,10 @@
       <c r="Z52" s="3"/>
     </row>
     <row r="53" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A53" s="86"/>
+      <c r="A53" s="85"/>
       <c r="B53" s="79"/>
       <c r="C53" s="79"/>
-      <c r="D53" s="86"/>
+      <c r="D53" s="85"/>
       <c r="E53" s="79"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -31603,19 +31609,19 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" ht="43.5" customHeight="1">
-      <c r="A54" s="87" t="s">
+      <c r="A54" s="86" t="s">
         <v>75</v>
       </c>
-      <c r="B54" s="82"/>
+      <c r="B54" s="81"/>
       <c r="C54" s="56" t="str">
-        <f>IF('Grading Sheet'!D25&gt;90,"A+",IF('Grading Sheet'!D25&gt;85,"A",IF('Grading Sheet'!D25&gt;80,"B+",IF('Grading Sheet'!D25&gt;75,"B",IF('Grading Sheet'!D25&gt;70,"C+",IF('Grading Sheet'!D25&gt;65,"C",IF('Grading Sheet'!D25&gt;60,"D+",IF('Grading Sheet'!D25&gt;55,"D",IF('Grading Sheet'!D25&gt;50,"E+",IF('Grading Sheet'!D25&gt;45,"F+","F"))))))))))</f>
-        <v>C</v>
+        <f>IF('Grading Sheet'!D25&gt;95,"A+",IF('Grading Sheet'!D25&gt;85,"A",IF('Grading Sheet'!D25&gt;75,"A-",IF('Grading Sheet'!D25&gt;67,"B+",IF('Grading Sheet'!D25&gt;63,"B",IF('Grading Sheet'!D25&gt;57,"C+",IF('Grading Sheet'!D25&gt;53,"C",IF('Grading Sheet'!D25&gt;47,"D+",IF('Grading Sheet'!D25&gt;43,"D",IF('Grading Sheet'!D25&gt;37,"F1","F2"))))))))))</f>
+        <v>B+</v>
       </c>
-      <c r="D54" s="89" t="str">
-        <f>IF('Grading Sheet'!D25&gt;90,"A+",IF('Grading Sheet'!D25&gt;85,"A",IF('Grading Sheet'!D25&gt;80,"B+",IF('Grading Sheet'!D25&gt;75,"B",IF('Grading Sheet'!D25&gt;70,"C+",IF('Grading Sheet'!D25&gt;65,"C",IF('Grading Sheet'!D25&gt;60,"D+",IF('Grading Sheet'!D25&gt;55,"D",IF('Grading Sheet'!D25&gt;50,"E+",IF('Grading Sheet'!D25&gt;45,"F+","F"))))))))))</f>
-        <v>C</v>
+      <c r="D54" s="88" t="str">
+        <f>IF('Grading Sheet'!D25&gt;95,"A+",IF('Grading Sheet'!D25&gt;85,"A",IF('Grading Sheet'!D25&gt;75,"A-",IF('Grading Sheet'!D25&gt;67,"B+",IF('Grading Sheet'!D25&gt;63,"B",IF('Grading Sheet'!D25&gt;57,"C+",IF('Grading Sheet'!D25&gt;53,"C",IF('Grading Sheet'!D25&gt;47,"D+",IF('Grading Sheet'!D25&gt;43,"D",IF('Grading Sheet'!D25&gt;37,"F1","F2"))))))))))</f>
+        <v>B+</v>
       </c>
-      <c r="E54" s="82"/>
+      <c r="E54" s="81"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -31639,7 +31645,7 @@
       <c r="Z54" s="3"/>
     </row>
     <row r="55" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A55" s="86"/>
+      <c r="A55" s="85"/>
       <c r="B55" s="79"/>
       <c r="C55" s="79"/>
       <c r="D55" s="79"/>
@@ -31667,13 +31673,13 @@
       <c r="Z55" s="3"/>
     </row>
     <row r="56" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A56" s="90" t="s">
+      <c r="A56" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="B56" s="91"/>
-      <c r="C56" s="91"/>
-      <c r="D56" s="91"/>
-      <c r="E56" s="91"/>
+      <c r="B56" s="90"/>
+      <c r="C56" s="90"/>
+      <c r="D56" s="90"/>
+      <c r="E56" s="90"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
@@ -31697,13 +31703,13 @@
       <c r="Z56" s="3"/>
     </row>
     <row r="57" spans="1:26" ht="112.5" customHeight="1">
-      <c r="A57" s="92" t="s">
+      <c r="A57" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="81"/>
-      <c r="C57" s="81"/>
-      <c r="D57" s="81"/>
-      <c r="E57" s="82"/>
+      <c r="B57" s="80"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="80"/>
+      <c r="E57" s="81"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -31727,13 +31733,13 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" ht="96" customHeight="1">
-      <c r="A58" s="80" t="s">
-        <v>89</v>
+      <c r="A58" s="106" t="s">
+        <v>97</v>
       </c>
-      <c r="B58" s="81"/>
-      <c r="C58" s="81"/>
-      <c r="D58" s="81"/>
-      <c r="E58" s="82"/>
+      <c r="B58" s="80"/>
+      <c r="C58" s="80"/>
+      <c r="D58" s="80"/>
+      <c r="E58" s="81"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>

</xml_diff>